<commit_message>
Additional logging. Recognize issue identifier row by content (don't automatically skip first row)
</commit_message>
<xml_diff>
--- a/goobi-plugin-administration-nli-dailypress/test/resources/DailyPress_SamplePapers.xlsx
+++ b/goobi-plugin-administration-nli-dailypress/test/resources/DailyPress_SamplePapers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t xml:space="preserve">CMS ID</t>
   </si>
@@ -77,14 +77,27 @@
   </si>
   <si>
     <t xml:space="preserve">Kleines Gemeindeblättchen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">003922137</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jerusalem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -151,8 +164,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -173,18 +190,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.5714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -208,7 +223,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1234</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -228,7 +243,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>5678</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -248,7 +263,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>9101</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -265,6 +280,23 @@
       </c>
       <c r="F4" s="0" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>